<commit_message>
importing pandas, had trouble with deep dive, maybe look at solution closely time permitting
</commit_message>
<xml_diff>
--- a/Data/Zipcode_Demos.xlsx
+++ b/Data/Zipcode_Demos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>Average Statistics</t>
   </si>
@@ -160,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +224,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -302,6 +307,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -336,6 +342,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,37 +518,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="32" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>10005.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>10005.799999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,7 +605,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -557,31 +613,31 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0.404</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -589,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -597,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -605,7 +661,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -613,7 +669,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -621,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -629,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -637,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -645,7 +701,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -653,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -661,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -669,7 +725,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -677,7 +733,7 @@
         <v>0.437</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -685,15 +741,15 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23">
-        <v>0.036</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -701,15 +757,15 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25">
-        <v>0.181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -717,7 +773,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -725,7 +781,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -733,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -741,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -749,15 +805,15 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B31">
-        <v>79.90000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>79.900000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -765,15 +821,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B33">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -781,15 +837,15 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B35">
-        <v>0.739</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -797,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -805,7 +861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -813,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -821,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -829,7 +885,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -837,15 +893,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B42">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -853,7 +909,7 @@
         <v>0.151</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -861,15 +917,15 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B45">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>0.64900000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -877,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -885,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -893,7 +949,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="49" spans="1:46">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:46">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>10001</v>
       </c>
@@ -1086,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="R50">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="S50">
         <v>1</v>
@@ -1104,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="X50">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Y50">
         <v>0</v>
@@ -1158,7 +1214,7 @@
         <v>24</v>
       </c>
       <c r="AP50">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AQ50">
         <v>0</v>
@@ -1173,7 +1229,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:46">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10002</v>
       </c>
@@ -1268,7 +1324,7 @@
         <v>33</v>
       </c>
       <c r="AF51">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -1298,7 +1354,7 @@
         <v>33</v>
       </c>
       <c r="AP51">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="AQ51">
         <v>0</v>
@@ -1313,7 +1369,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:46">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>10003</v>
       </c>
@@ -1453,7 +1509,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:46">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>10004</v>
       </c>
@@ -1593,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:46">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>10005</v>
       </c>
@@ -1733,7 +1789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:46">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>10006</v>
       </c>
@@ -1873,7 +1929,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:46">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>10007</v>
       </c>
@@ -2013,7 +2069,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:46">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>10009</v>
       </c>
@@ -2153,7 +2209,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:46">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>10010</v>
       </c>
@@ -2293,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:46">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>10011</v>
       </c>

</xml_diff>